<commit_message>
DS hanghoa: add column {TonToiThieu, ChenhLech}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_DanhMucHangHoa.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_DanhMucHangHoa.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Trạng thái</t>
   </si>
@@ -46,13 +46,16 @@
     <t>BẢNG TỔNG HỢP DANH MỤC HÀNG HÓA</t>
   </si>
   <si>
-    <t xml:space="preserve">Tổng cộng: </t>
-  </si>
-  <si>
     <t>ĐVT</t>
   </si>
   <si>
     <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>Tồn tối thiểu</t>
+  </si>
+  <si>
+    <t>Chênh lệch</t>
   </si>
 </sst>
 </file>
@@ -62,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,16 +93,8 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,13 +106,8 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -140,65 +130,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -228,32 +165,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -555,43 +476,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="11" customWidth="1"/>
     <col min="4" max="4" width="34.5703125" style="7" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" style="7" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" style="9" customWidth="1"/>
-    <col min="8" max="9" width="15.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="9" width="14.7109375" style="9" customWidth="1"/>
+    <col min="10" max="11" width="15.7109375" style="9" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="5"/>
-    </row>
-    <row r="3" spans="1:11" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="5"/>
+    </row>
+    <row r="3" spans="1:13" s="10" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -599,7 +522,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>3</v>
@@ -619,11 +542,17 @@
       <c r="I3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="6"/>
       <c r="C4" s="2"/>
@@ -633,9 +562,11 @@
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="6"/>
       <c r="C5" s="2"/>
@@ -645,9 +576,11 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="6"/>
       <c r="C6" s="2"/>
@@ -657,9 +590,11 @@
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="6"/>
       <c r="C7" s="2"/>
@@ -669,9 +604,11 @@
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="6"/>
       <c r="C8" s="2"/>
@@ -681,9 +618,11 @@
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="6"/>
       <c r="C9" s="2"/>
@@ -693,9 +632,11 @@
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="6"/>
       <c r="C10" s="2"/>
@@ -705,9 +646,11 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="6"/>
       <c r="C11" s="2"/>
@@ -717,9 +660,11 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="6"/>
       <c r="C12" s="2"/>
@@ -729,9 +674,11 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="6"/>
       <c r="C13" s="2"/>
@@ -741,9 +688,11 @@
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="6"/>
       <c r="C14" s="2"/>
@@ -753,9 +702,11 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="6"/>
       <c r="C15" s="2"/>
@@ -765,9 +716,11 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="6"/>
       <c r="C16" s="2"/>
@@ -777,9 +730,11 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="6"/>
       <c r="C17" s="2"/>
@@ -789,9 +744,11 @@
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="6"/>
       <c r="C18" s="2"/>
@@ -801,9 +758,11 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="6"/>
       <c r="C19" s="2"/>
@@ -813,9 +772,11 @@
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="6"/>
       <c r="C20" s="2"/>
@@ -825,9 +786,11 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="6"/>
       <c r="C21" s="2"/>
@@ -837,9 +800,11 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="6"/>
       <c r="C22" s="2"/>
@@ -849,9 +814,11 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="6"/>
       <c r="C23" s="2"/>
@@ -861,9 +828,11 @@
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="6"/>
       <c r="C24" s="2"/>
@@ -873,9 +842,11 @@
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="6"/>
       <c r="C25" s="2"/>
@@ -885,9 +856,11 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="6"/>
       <c r="C26" s="2"/>
@@ -897,9 +870,11 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="6"/>
       <c r="C27" s="2"/>
@@ -909,29 +884,13 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="12">
-        <f>SUM($H$4:H27)</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="12"/>
-      <c r="J28" s="11"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A28:G28"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>